<commit_message>
Corrección de imágenes de camisas
Quitado del logo.
</commit_message>
<xml_diff>
--- a/Producteca_img.xlsx
+++ b/Producteca_img.xlsx
@@ -4170,8 +4170,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I2523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2062" workbookViewId="0">
-      <selection activeCell="D2111" sqref="D2111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62125,7 +62125,7 @@
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1"/>
     <hyperlink ref="F17" r:id="rId2"/>
-    <hyperlink ref="F2105"/>
+    <hyperlink ref="F2105" display="https://raw.githubusercontent.com/edgardoraul/imagenes_rerda/main/1120330/1.jpg,https://raw.githubusercontent.com/edgardoraul/imagenes_rerda/main/1120330/2.jpg,https://raw.githubusercontent.com/edgardoraul/imagenes_rerda/main/1120330/3.jpg,https://raw.git"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>

</xml_diff>